<commit_message>
check 14 including leadership
</commit_message>
<xml_diff>
--- a/Quality reports shared/tools difference.xlsx
+++ b/Quality reports shared/tools difference.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="57">
   <si>
     <t>district_name</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Nganiko</t>
   </si>
   <si>
-    <t>Nyakacwamba</t>
-  </si>
-  <si>
     <t>Kanoni</t>
   </si>
   <si>
@@ -61,21 +58,9 @@
     <t>Kyamakanaga</t>
   </si>
   <si>
-    <t>Bujumiro_A</t>
-  </si>
-  <si>
-    <t>Bujumiro_B</t>
-  </si>
-  <si>
     <t>Kanyamburara</t>
   </si>
   <si>
-    <t>Kyarubingo</t>
-  </si>
-  <si>
-    <t>Nyabwina_Buhanda</t>
-  </si>
-  <si>
     <t>Muyenga_Central</t>
   </si>
   <si>
@@ -85,9 +70,6 @@
     <t>Nganiko_2</t>
   </si>
   <si>
-    <t>Nganiko_3</t>
-  </si>
-  <si>
     <t>Zanzibar</t>
   </si>
   <si>
@@ -115,30 +97,6 @@
     <t>Nganiko_TC</t>
   </si>
   <si>
-    <t>Kapapari</t>
-  </si>
-  <si>
-    <t>Karere_Nyakacwamba</t>
-  </si>
-  <si>
-    <t>Karubuguma_1</t>
-  </si>
-  <si>
-    <t>Karubuguma_2</t>
-  </si>
-  <si>
-    <t>Mpanga_Nyakacwamba</t>
-  </si>
-  <si>
-    <t>Nyakacwamba_1</t>
-  </si>
-  <si>
-    <t>Nyakacwamba_2</t>
-  </si>
-  <si>
-    <t>Rwengwe_Nyakacwamba</t>
-  </si>
-  <si>
     <t>Kanoni_Rakai</t>
   </si>
   <si>
@@ -181,34 +139,34 @@
     <t>Nnongo_A</t>
   </si>
   <si>
+    <t>Compound Sacks</t>
+  </si>
+  <si>
+    <t>Filters</t>
+  </si>
+  <si>
+    <t>Forked Hoe</t>
+  </si>
+  <si>
+    <t>Gloves</t>
+  </si>
+  <si>
+    <t>Hoes</t>
+  </si>
+  <si>
+    <t>Jerrycans</t>
+  </si>
+  <si>
+    <t>Mortar and Pestle</t>
+  </si>
+  <si>
+    <t>Pick Axe</t>
+  </si>
+  <si>
+    <t>Plastic Drums</t>
+  </si>
+  <si>
     <t>Pruning saw</t>
-  </si>
-  <si>
-    <t>Compound Sacks</t>
-  </si>
-  <si>
-    <t>Filters</t>
-  </si>
-  <si>
-    <t>Forked Hoe</t>
-  </si>
-  <si>
-    <t>Gloves</t>
-  </si>
-  <si>
-    <t>Hoes</t>
-  </si>
-  <si>
-    <t>Jerrycans</t>
-  </si>
-  <si>
-    <t>Mortar and Pestle</t>
-  </si>
-  <si>
-    <t>Pick Axe</t>
-  </si>
-  <si>
-    <t>Plastic Drums</t>
   </si>
   <si>
     <t>Secateurs</t>
@@ -584,7 +542,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -618,13 +576,16 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>41</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
       </c>
       <c r="F2">
-        <v>60</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -635,13 +596,16 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>42</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
       </c>
       <c r="F3">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -652,10 +616,10 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E4">
         <v>7</v>
@@ -672,16 +636,16 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F5">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -692,16 +656,16 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F6">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -712,10 +676,10 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E7">
         <v>14</v>
@@ -732,16 +696,16 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E8">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F8">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -752,16 +716,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="E9">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F9">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -772,10 +736,10 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E10">
         <v>7</v>
@@ -792,16 +756,16 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E11">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="F11">
-        <v>8</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -812,16 +776,16 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E12">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="F12">
-        <v>8</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -832,13 +796,16 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="E13">
+        <v>14</v>
       </c>
       <c r="F13">
-        <v>80</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -849,16 +816,16 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E14">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="F14">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -869,16 +836,16 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E15">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="F15">
-        <v>16</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -889,16 +856,16 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E16">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="F16">
-        <v>8</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -906,19 +873,16 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F17">
-        <v>80</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -926,19 +890,19 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="E18">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="F18">
-        <v>40</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -946,16 +910,16 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F19">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -963,16 +927,16 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F20">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -983,13 +947,13 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F21">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -997,16 +961,16 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22">
         <v>20</v>
-      </c>
-      <c r="D22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22">
-        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1014,19 +978,16 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="F23">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1034,16 +995,16 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
         <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F24">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1051,13 +1012,13 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1068,16 +1029,16 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F26">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1085,13 +1046,13 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1102,16 +1063,16 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F28">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1119,30 +1080,30 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F29">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1150,50 +1111,50 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F31">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F32">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -1201,33 +1162,33 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F34">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1235,33 +1196,33 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F36">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D37" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1269,33 +1230,33 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D38" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F38">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D39" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1303,33 +1264,33 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F40">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -1337,443 +1298,35 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C42" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F42">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D43" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
-        <v>32</v>
-      </c>
-      <c r="D44" t="s">
-        <v>55</v>
-      </c>
-      <c r="F44">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" t="s">
-        <v>70</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" t="s">
-        <v>6</v>
-      </c>
-      <c r="B46" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" t="s">
-        <v>55</v>
-      </c>
-      <c r="F46">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" t="s">
-        <v>11</v>
-      </c>
-      <c r="C47" t="s">
-        <v>34</v>
-      </c>
-      <c r="D47" t="s">
-        <v>55</v>
-      </c>
-      <c r="F47">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" t="s">
-        <v>35</v>
-      </c>
-      <c r="D48" t="s">
-        <v>55</v>
-      </c>
-      <c r="F48">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" t="s">
-        <v>11</v>
-      </c>
-      <c r="C49" t="s">
-        <v>36</v>
-      </c>
-      <c r="D49" t="s">
-        <v>55</v>
-      </c>
-      <c r="F49">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" t="s">
-        <v>6</v>
-      </c>
-      <c r="B50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" t="s">
-        <v>37</v>
-      </c>
-      <c r="D50" t="s">
-        <v>55</v>
-      </c>
-      <c r="F50">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" t="s">
-        <v>6</v>
-      </c>
-      <c r="B51" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" t="s">
-        <v>38</v>
-      </c>
-      <c r="D51" t="s">
-        <v>55</v>
-      </c>
-      <c r="F51">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" t="s">
-        <v>6</v>
-      </c>
-      <c r="B52" t="s">
-        <v>11</v>
-      </c>
-      <c r="C52" t="s">
-        <v>39</v>
-      </c>
-      <c r="D52" t="s">
-        <v>55</v>
-      </c>
-      <c r="F52">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" t="s">
-        <v>40</v>
-      </c>
-      <c r="D53" t="s">
-        <v>55</v>
-      </c>
-      <c r="F53">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" t="s">
-        <v>7</v>
-      </c>
-      <c r="B54" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54" t="s">
-        <v>41</v>
-      </c>
-      <c r="D54" t="s">
-        <v>70</v>
-      </c>
-      <c r="F54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" t="s">
-        <v>7</v>
-      </c>
-      <c r="B55" t="s">
-        <v>12</v>
-      </c>
-      <c r="C55" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" t="s">
-        <v>70</v>
-      </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" t="s">
-        <v>7</v>
-      </c>
-      <c r="B56" t="s">
-        <v>12</v>
-      </c>
-      <c r="C56" t="s">
-        <v>43</v>
-      </c>
-      <c r="D56" t="s">
-        <v>70</v>
-      </c>
-      <c r="F56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" t="s">
-        <v>7</v>
-      </c>
-      <c r="B57" t="s">
-        <v>13</v>
-      </c>
-      <c r="C57" t="s">
-        <v>44</v>
-      </c>
-      <c r="D57" t="s">
-        <v>70</v>
-      </c>
-      <c r="F57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" t="s">
-        <v>7</v>
-      </c>
-      <c r="B58" t="s">
-        <v>13</v>
-      </c>
-      <c r="C58" t="s">
-        <v>45</v>
-      </c>
-      <c r="D58" t="s">
-        <v>70</v>
-      </c>
-      <c r="F58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" t="s">
-        <v>7</v>
-      </c>
-      <c r="B59" t="s">
-        <v>13</v>
-      </c>
-      <c r="C59" t="s">
-        <v>46</v>
-      </c>
-      <c r="D59" t="s">
-        <v>70</v>
-      </c>
-      <c r="F59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" t="s">
-        <v>7</v>
-      </c>
-      <c r="B60" t="s">
-        <v>13</v>
-      </c>
-      <c r="C60" t="s">
-        <v>47</v>
-      </c>
-      <c r="D60" t="s">
-        <v>70</v>
-      </c>
-      <c r="F60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" t="s">
-        <v>7</v>
-      </c>
-      <c r="B61" t="s">
-        <v>13</v>
-      </c>
-      <c r="C61" t="s">
-        <v>48</v>
-      </c>
-      <c r="D61" t="s">
-        <v>70</v>
-      </c>
-      <c r="F61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" t="s">
-        <v>7</v>
-      </c>
-      <c r="B62" t="s">
-        <v>13</v>
-      </c>
-      <c r="C62" t="s">
-        <v>49</v>
-      </c>
-      <c r="D62" t="s">
-        <v>70</v>
-      </c>
-      <c r="F62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" t="s">
-        <v>7</v>
-      </c>
-      <c r="B63" t="s">
-        <v>13</v>
-      </c>
-      <c r="C63" t="s">
-        <v>50</v>
-      </c>
-      <c r="D63" t="s">
-        <v>70</v>
-      </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" t="s">
-        <v>7</v>
-      </c>
-      <c r="B64" t="s">
-        <v>13</v>
-      </c>
-      <c r="C64" t="s">
-        <v>51</v>
-      </c>
-      <c r="D64" t="s">
-        <v>70</v>
-      </c>
-      <c r="F64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" t="s">
-        <v>7</v>
-      </c>
-      <c r="B65" t="s">
-        <v>13</v>
-      </c>
-      <c r="C65" t="s">
-        <v>52</v>
-      </c>
-      <c r="D65" t="s">
-        <v>70</v>
-      </c>
-      <c r="F65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" t="s">
-        <v>7</v>
-      </c>
-      <c r="B66" t="s">
-        <v>14</v>
-      </c>
-      <c r="C66" t="s">
-        <v>53</v>
-      </c>
-      <c r="D66" t="s">
-        <v>70</v>
-      </c>
-      <c r="F66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" t="s">
-        <v>7</v>
-      </c>
-      <c r="B67" t="s">
-        <v>14</v>
-      </c>
-      <c r="C67" t="s">
-        <v>54</v>
-      </c>
-      <c r="D67" t="s">
-        <v>70</v>
-      </c>
-      <c r="F67">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add coffee pest and disease mgt
</commit_message>
<xml_diff>
--- a/Quality reports shared/tools difference.xlsx
+++ b/Quality reports shared/tools difference.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="56">
   <si>
     <t>district_name</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Zanzibar</t>
-  </si>
-  <si>
-    <t>Kagorogoro_A</t>
   </si>
   <si>
     <t>Kagorogoro_B</t>
@@ -542,7 +539,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -579,7 +576,7 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2">
         <v>7</v>
@@ -599,7 +596,7 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3">
         <v>7</v>
@@ -619,7 +616,7 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4">
         <v>7</v>
@@ -639,7 +636,7 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5">
         <v>14</v>
@@ -659,7 +656,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6">
         <v>14</v>
@@ -679,7 +676,7 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7">
         <v>14</v>
@@ -699,7 +696,7 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8">
         <v>7</v>
@@ -719,7 +716,7 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -739,7 +736,7 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10">
         <v>7</v>
@@ -759,7 +756,7 @@
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11">
         <v>70</v>
@@ -779,7 +776,7 @@
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E12">
         <v>35</v>
@@ -799,7 +796,7 @@
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13">
         <v>14</v>
@@ -819,7 +816,7 @@
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14">
         <v>7</v>
@@ -839,7 +836,7 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15">
         <v>70</v>
@@ -859,7 +856,7 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16">
         <v>35</v>
@@ -879,7 +876,7 @@
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F17">
         <v>2</v>
@@ -896,7 +893,7 @@
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18">
         <v>6</v>
@@ -916,7 +913,7 @@
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -933,7 +930,7 @@
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -950,7 +947,7 @@
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -967,10 +964,10 @@
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F22">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -984,7 +981,7 @@
         <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1001,7 +998,7 @@
         <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1018,7 +1015,7 @@
         <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1035,7 +1032,7 @@
         <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1052,7 +1049,7 @@
         <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1069,7 +1066,7 @@
         <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -1077,16 +1074,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C29" t="s">
         <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -1103,7 +1100,7 @@
         <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1120,7 +1117,7 @@
         <v>28</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1131,13 +1128,13 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C32" t="s">
         <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1154,7 +1151,7 @@
         <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -1171,7 +1168,7 @@
         <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1188,7 +1185,7 @@
         <v>32</v>
       </c>
       <c r="D35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1205,7 +1202,7 @@
         <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -1222,7 +1219,7 @@
         <v>34</v>
       </c>
       <c r="D37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1239,7 +1236,7 @@
         <v>35</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1256,7 +1253,7 @@
         <v>36</v>
       </c>
       <c r="D39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1273,7 +1270,7 @@
         <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -1284,13 +1281,13 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C41" t="s">
         <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -1307,26 +1304,9 @@
         <v>39</v>
       </c>
       <c r="D42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C43" t="s">
-        <v>40</v>
-      </c>
-      <c r="D43" t="s">
-        <v>56</v>
-      </c>
-      <c r="F43">
         <v>0</v>
       </c>
     </row>

</xml_diff>